<commit_message>
added blank spaces to end of abbrs
</commit_message>
<xml_diff>
--- a/abbrs.xlsx
+++ b/abbrs.xlsx
@@ -1802,7 +1802,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1812,7 +1812,6 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -1828,14 +1827,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -5301,7 +5297,7 @@
       <c r="B153" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C153" s="3" t="s">
+      <c r="C153" s="2" t="s">
         <v>297</v>
       </c>
     </row>
@@ -6981,319 +6977,1543 @@
       <c r="A306" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="B306" s="3" t="s">
+      <c r="B306" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="C306" s="3" t="s">
+      <c r="C306" s="2" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
-    <row r="340" ht="15.75" customHeight="1"/>
-    <row r="341" ht="15.75" customHeight="1"/>
-    <row r="342" ht="15.75" customHeight="1"/>
-    <row r="343" ht="15.75" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
-    <row r="349" ht="15.75" customHeight="1"/>
-    <row r="350" ht="15.75" customHeight="1"/>
-    <row r="351" ht="15.75" customHeight="1"/>
-    <row r="352" ht="15.75" customHeight="1"/>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
-    <row r="369" ht="15.75" customHeight="1"/>
-    <row r="370" ht="15.75" customHeight="1"/>
-    <row r="371" ht="15.75" customHeight="1"/>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
-    <row r="417" ht="15.75" customHeight="1"/>
-    <row r="418" ht="15.75" customHeight="1"/>
-    <row r="419" ht="15.75" customHeight="1"/>
-    <row r="420" ht="15.75" customHeight="1"/>
-    <row r="421" ht="15.75" customHeight="1"/>
-    <row r="422" ht="15.75" customHeight="1"/>
-    <row r="423" ht="15.75" customHeight="1"/>
-    <row r="424" ht="15.75" customHeight="1"/>
-    <row r="425" ht="15.75" customHeight="1"/>
-    <row r="426" ht="15.75" customHeight="1"/>
-    <row r="427" ht="15.75" customHeight="1"/>
-    <row r="428" ht="15.75" customHeight="1"/>
-    <row r="429" ht="15.75" customHeight="1"/>
-    <row r="430" ht="15.75" customHeight="1"/>
-    <row r="431" ht="15.75" customHeight="1"/>
-    <row r="432" ht="15.75" customHeight="1"/>
-    <row r="433" ht="15.75" customHeight="1"/>
-    <row r="434" ht="15.75" customHeight="1"/>
-    <row r="435" ht="15.75" customHeight="1"/>
-    <row r="436" ht="15.75" customHeight="1"/>
-    <row r="437" ht="15.75" customHeight="1"/>
-    <row r="438" ht="15.75" customHeight="1"/>
-    <row r="439" ht="15.75" customHeight="1"/>
-    <row r="440" ht="15.75" customHeight="1"/>
-    <row r="441" ht="15.75" customHeight="1"/>
-    <row r="442" ht="15.75" customHeight="1"/>
-    <row r="443" ht="15.75" customHeight="1"/>
-    <row r="444" ht="15.75" customHeight="1"/>
-    <row r="445" ht="15.75" customHeight="1"/>
-    <row r="446" ht="15.75" customHeight="1"/>
-    <row r="447" ht="15.75" customHeight="1"/>
-    <row r="448" ht="15.75" customHeight="1"/>
-    <row r="449" ht="15.75" customHeight="1"/>
-    <row r="450" ht="15.75" customHeight="1"/>
-    <row r="451" ht="15.75" customHeight="1"/>
-    <row r="452" ht="15.75" customHeight="1"/>
-    <row r="453" ht="15.75" customHeight="1"/>
-    <row r="454" ht="15.75" customHeight="1"/>
-    <row r="455" ht="15.75" customHeight="1"/>
-    <row r="456" ht="15.75" customHeight="1"/>
-    <row r="457" ht="15.75" customHeight="1"/>
-    <row r="458" ht="15.75" customHeight="1"/>
-    <row r="459" ht="15.75" customHeight="1"/>
-    <row r="460" ht="15.75" customHeight="1"/>
-    <row r="461" ht="15.75" customHeight="1"/>
-    <row r="462" ht="15.75" customHeight="1"/>
-    <row r="463" ht="15.75" customHeight="1"/>
-    <row r="464" ht="15.75" customHeight="1"/>
-    <row r="465" ht="15.75" customHeight="1"/>
-    <row r="466" ht="15.75" customHeight="1"/>
-    <row r="467" ht="15.75" customHeight="1"/>
-    <row r="468" ht="15.75" customHeight="1"/>
-    <row r="469" ht="15.75" customHeight="1"/>
-    <row r="470" ht="15.75" customHeight="1"/>
-    <row r="471" ht="15.75" customHeight="1"/>
-    <row r="472" ht="15.75" customHeight="1"/>
-    <row r="473" ht="15.75" customHeight="1"/>
-    <row r="474" ht="15.75" customHeight="1"/>
-    <row r="475" ht="15.75" customHeight="1"/>
-    <row r="476" ht="15.75" customHeight="1"/>
-    <row r="477" ht="15.75" customHeight="1"/>
-    <row r="478" ht="15.75" customHeight="1"/>
-    <row r="479" ht="15.75" customHeight="1"/>
-    <row r="480" ht="15.75" customHeight="1"/>
-    <row r="481" ht="15.75" customHeight="1"/>
-    <row r="482" ht="15.75" customHeight="1"/>
-    <row r="483" ht="15.75" customHeight="1"/>
-    <row r="484" ht="15.75" customHeight="1"/>
-    <row r="485" ht="15.75" customHeight="1"/>
-    <row r="486" ht="15.75" customHeight="1"/>
-    <row r="487" ht="15.75" customHeight="1"/>
-    <row r="488" ht="15.75" customHeight="1"/>
-    <row r="489" ht="15.75" customHeight="1"/>
-    <row r="490" ht="15.75" customHeight="1"/>
-    <row r="491" ht="15.75" customHeight="1"/>
-    <row r="492" ht="15.75" customHeight="1"/>
-    <row r="493" ht="15.75" customHeight="1"/>
-    <row r="494" ht="15.75" customHeight="1"/>
-    <row r="495" ht="15.75" customHeight="1"/>
-    <row r="496" ht="15.75" customHeight="1"/>
-    <row r="497" ht="15.75" customHeight="1"/>
-    <row r="498" ht="15.75" customHeight="1"/>
-    <row r="499" ht="15.75" customHeight="1"/>
-    <row r="500" ht="15.75" customHeight="1"/>
-    <row r="501" ht="15.75" customHeight="1"/>
-    <row r="502" ht="15.75" customHeight="1"/>
-    <row r="503" ht="15.75" customHeight="1"/>
-    <row r="504" ht="15.75" customHeight="1"/>
-    <row r="505" ht="15.75" customHeight="1"/>
-    <row r="506" ht="15.75" customHeight="1"/>
-    <row r="507" ht="15.75" customHeight="1"/>
-    <row r="508" ht="15.75" customHeight="1"/>
-    <row r="509" ht="15.75" customHeight="1"/>
-    <row r="510" ht="15.75" customHeight="1"/>
-    <row r="511" ht="15.75" customHeight="1"/>
-    <row r="512" ht="15.75" customHeight="1"/>
-    <row r="513" ht="15.75" customHeight="1"/>
-    <row r="514" ht="15.75" customHeight="1"/>
-    <row r="515" ht="15.75" customHeight="1"/>
-    <row r="516" ht="15.75" customHeight="1"/>
-    <row r="517" ht="15.75" customHeight="1"/>
-    <row r="518" ht="15.75" customHeight="1"/>
-    <row r="519" ht="15.75" customHeight="1"/>
-    <row r="520" ht="15.75" customHeight="1"/>
-    <row r="521" ht="15.75" customHeight="1"/>
-    <row r="522" ht="15.75" customHeight="1"/>
-    <row r="523" ht="15.75" customHeight="1"/>
-    <row r="524" ht="15.75" customHeight="1"/>
-    <row r="525" ht="15.75" customHeight="1"/>
-    <row r="526" ht="15.75" customHeight="1"/>
-    <row r="527" ht="15.75" customHeight="1"/>
-    <row r="528" ht="15.75" customHeight="1"/>
-    <row r="529" ht="15.75" customHeight="1"/>
-    <row r="530" ht="15.75" customHeight="1"/>
-    <row r="531" ht="15.75" customHeight="1"/>
-    <row r="532" ht="15.75" customHeight="1"/>
-    <row r="533" ht="15.75" customHeight="1"/>
-    <row r="534" ht="15.75" customHeight="1"/>
-    <row r="535" ht="15.75" customHeight="1"/>
-    <row r="536" ht="15.75" customHeight="1"/>
-    <row r="537" ht="15.75" customHeight="1"/>
-    <row r="538" ht="15.75" customHeight="1"/>
-    <row r="539" ht="15.75" customHeight="1"/>
-    <row r="540" ht="15.75" customHeight="1"/>
-    <row r="541" ht="15.75" customHeight="1"/>
-    <row r="542" ht="15.75" customHeight="1"/>
-    <row r="543" ht="15.75" customHeight="1"/>
-    <row r="544" ht="15.75" customHeight="1"/>
-    <row r="545" ht="15.75" customHeight="1"/>
-    <row r="546" ht="15.75" customHeight="1"/>
-    <row r="547" ht="15.75" customHeight="1"/>
-    <row r="548" ht="15.75" customHeight="1"/>
-    <row r="549" ht="15.75" customHeight="1"/>
-    <row r="550" ht="15.75" customHeight="1"/>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1">
+      <c r="A307" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="308" ht="15.75" customHeight="1">
+      <c r="A308" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" ht="15.75" customHeight="1">
+      <c r="A309" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="310" ht="15.75" customHeight="1">
+      <c r="A310" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311" ht="15.75" customHeight="1">
+      <c r="A311" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" ht="15.75" customHeight="1">
+      <c r="A312" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" ht="15.75" customHeight="1">
+      <c r="A313" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" ht="15.75" customHeight="1">
+      <c r="A314" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" ht="15.75" customHeight="1">
+      <c r="A315" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" ht="15.75" customHeight="1">
+      <c r="A316" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317" ht="15.75" customHeight="1">
+      <c r="A317" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="318" ht="15.75" customHeight="1">
+      <c r="A318" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="319" ht="15.75" customHeight="1">
+      <c r="A319" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320" ht="15.75" customHeight="1">
+      <c r="A320" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="321" ht="15.75" customHeight="1">
+      <c r="A321" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="322" ht="15.75" customHeight="1">
+      <c r="A322" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="323" ht="15.75" customHeight="1">
+      <c r="A323" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" ht="15.75" customHeight="1">
+      <c r="A324" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="325" ht="15.75" customHeight="1">
+      <c r="A325" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="326" ht="15.75" customHeight="1">
+      <c r="A326" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="327" ht="15.75" customHeight="1">
+      <c r="A327" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="328" ht="15.75" customHeight="1">
+      <c r="A328" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="329" ht="15.75" customHeight="1">
+      <c r="A329" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="330" ht="15.75" customHeight="1">
+      <c r="A330" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="331" ht="15.75" customHeight="1">
+      <c r="A331" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="332" ht="15.75" customHeight="1">
+      <c r="A332" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="333" ht="15.75" customHeight="1">
+      <c r="A333" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="334" ht="15.75" customHeight="1">
+      <c r="A334" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="335" ht="15.75" customHeight="1">
+      <c r="A335" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="336" ht="15.75" customHeight="1">
+      <c r="A336" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="337" ht="15.75" customHeight="1">
+      <c r="A337" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="338" ht="15.75" customHeight="1">
+      <c r="A338" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="339" ht="15.75" customHeight="1">
+      <c r="A339" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="340" ht="15.75" customHeight="1">
+      <c r="A340" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="341" ht="15.75" customHeight="1">
+      <c r="A341" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="342" ht="15.75" customHeight="1">
+      <c r="A342" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="343" ht="15.75" customHeight="1">
+      <c r="A343" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="344" ht="15.75" customHeight="1">
+      <c r="A344" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="345" ht="15.75" customHeight="1">
+      <c r="A345" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="346" ht="15.75" customHeight="1">
+      <c r="A346" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="347" ht="15.75" customHeight="1">
+      <c r="A347" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="348" ht="15.75" customHeight="1">
+      <c r="A348" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="349" ht="15.75" customHeight="1">
+      <c r="A349" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="350" ht="15.75" customHeight="1">
+      <c r="A350" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="351" ht="15.75" customHeight="1">
+      <c r="A351" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="352" ht="15.75" customHeight="1">
+      <c r="A352" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="353" ht="15.75" customHeight="1">
+      <c r="A353" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="354" ht="15.75" customHeight="1">
+      <c r="A354" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="355" ht="15.75" customHeight="1">
+      <c r="A355" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="356" ht="15.75" customHeight="1">
+      <c r="A356" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="357" ht="15.75" customHeight="1">
+      <c r="A357" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="358" ht="15.75" customHeight="1">
+      <c r="A358" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="359" ht="15.75" customHeight="1">
+      <c r="A359" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="360" ht="15.75" customHeight="1">
+      <c r="A360" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="361" ht="15.75" customHeight="1">
+      <c r="A361" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="362" ht="15.75" customHeight="1">
+      <c r="A362" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="363" ht="15.75" customHeight="1">
+      <c r="A363" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="364" ht="15.75" customHeight="1">
+      <c r="A364" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="365" ht="15.75" customHeight="1">
+      <c r="A365" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="366" ht="15.75" customHeight="1">
+      <c r="A366" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="367" ht="15.75" customHeight="1">
+      <c r="A367" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="368" ht="15.75" customHeight="1">
+      <c r="A368" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="369" ht="15.75" customHeight="1">
+      <c r="A369" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="370" ht="15.75" customHeight="1">
+      <c r="A370" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="371" ht="15.75" customHeight="1">
+      <c r="A371" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="372" ht="15.75" customHeight="1">
+      <c r="A372" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="373" ht="15.75" customHeight="1">
+      <c r="A373" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="374" ht="15.75" customHeight="1">
+      <c r="A374" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="375" ht="15.75" customHeight="1">
+      <c r="A375" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="376" ht="15.75" customHeight="1">
+      <c r="A376" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="377" ht="15.75" customHeight="1">
+      <c r="A377" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="378" ht="15.75" customHeight="1">
+      <c r="A378" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="379" ht="15.75" customHeight="1">
+      <c r="A379" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="380" ht="15.75" customHeight="1">
+      <c r="A380" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="381" ht="15.75" customHeight="1">
+      <c r="A381" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="382" ht="15.75" customHeight="1">
+      <c r="A382" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="383" ht="15.75" customHeight="1">
+      <c r="A383" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="384" ht="15.75" customHeight="1">
+      <c r="A384" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="385" ht="15.75" customHeight="1">
+      <c r="A385" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="386" ht="15.75" customHeight="1">
+      <c r="A386" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="387" ht="15.75" customHeight="1">
+      <c r="A387" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="388" ht="15.75" customHeight="1">
+      <c r="A388" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="389" ht="15.75" customHeight="1">
+      <c r="A389" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="390" ht="15.75" customHeight="1">
+      <c r="A390" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="391" ht="15.75" customHeight="1">
+      <c r="A391" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="392" ht="15.75" customHeight="1">
+      <c r="A392" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="393" ht="15.75" customHeight="1">
+      <c r="A393" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="394" ht="15.75" customHeight="1">
+      <c r="A394" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="395" ht="15.75" customHeight="1">
+      <c r="A395" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="396" ht="15.75" customHeight="1">
+      <c r="A396" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="397" ht="15.75" customHeight="1">
+      <c r="A397" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="398" ht="15.75" customHeight="1">
+      <c r="A398" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="399" ht="15.75" customHeight="1">
+      <c r="A399" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="400" ht="15.75" customHeight="1">
+      <c r="A400" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="401" ht="15.75" customHeight="1">
+      <c r="A401" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="402" ht="15.75" customHeight="1">
+      <c r="A402" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="403" ht="15.75" customHeight="1">
+      <c r="A403" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="404" ht="15.75" customHeight="1">
+      <c r="A404" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="405" ht="15.75" customHeight="1">
+      <c r="A405" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="406" ht="15.75" customHeight="1">
+      <c r="A406" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="407" ht="15.75" customHeight="1">
+      <c r="A407" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="408" ht="15.75" customHeight="1">
+      <c r="A408" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="409" ht="15.75" customHeight="1">
+      <c r="A409" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="410" ht="15.75" customHeight="1">
+      <c r="A410" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="411" ht="15.75" customHeight="1">
+      <c r="A411" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="412" ht="15.75" customHeight="1">
+      <c r="A412" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="413" ht="15.75" customHeight="1">
+      <c r="A413" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="414" ht="15.75" customHeight="1">
+      <c r="A414" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="415" ht="15.75" customHeight="1">
+      <c r="A415" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="416" ht="15.75" customHeight="1">
+      <c r="A416" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="417" ht="15.75" customHeight="1">
+      <c r="A417" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="418" ht="15.75" customHeight="1">
+      <c r="A418" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="419" ht="15.75" customHeight="1">
+      <c r="A419" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="420" ht="15.75" customHeight="1">
+      <c r="A420" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="421" ht="15.75" customHeight="1">
+      <c r="A421" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="422" ht="15.75" customHeight="1">
+      <c r="A422" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="423" ht="15.75" customHeight="1">
+      <c r="A423" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="424" ht="15.75" customHeight="1">
+      <c r="A424" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="425" ht="15.75" customHeight="1">
+      <c r="A425" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="426" ht="15.75" customHeight="1">
+      <c r="A426" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="427" ht="15.75" customHeight="1">
+      <c r="A427" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="428" ht="15.75" customHeight="1">
+      <c r="A428" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="429" ht="15.75" customHeight="1">
+      <c r="A429" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="430" ht="15.75" customHeight="1">
+      <c r="A430" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="431" ht="15.75" customHeight="1">
+      <c r="A431" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="432" ht="15.75" customHeight="1">
+      <c r="A432" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="433" ht="15.75" customHeight="1">
+      <c r="A433" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="434" ht="15.75" customHeight="1">
+      <c r="A434" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="435" ht="15.75" customHeight="1">
+      <c r="A435" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="436" ht="15.75" customHeight="1">
+      <c r="A436" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="437" ht="15.75" customHeight="1">
+      <c r="A437" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="438" ht="15.75" customHeight="1">
+      <c r="A438" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="439" ht="15.75" customHeight="1">
+      <c r="A439" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="440" ht="15.75" customHeight="1">
+      <c r="A440" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="441" ht="15.75" customHeight="1">
+      <c r="A441" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="442" ht="15.75" customHeight="1">
+      <c r="A442" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="443" ht="15.75" customHeight="1">
+      <c r="A443" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="444" ht="15.75" customHeight="1">
+      <c r="A444" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="445" ht="15.75" customHeight="1">
+      <c r="A445" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="446" ht="15.75" customHeight="1">
+      <c r="A446" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="447" ht="15.75" customHeight="1">
+      <c r="A447" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="448" ht="15.75" customHeight="1">
+      <c r="A448" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="449" ht="15.75" customHeight="1">
+      <c r="A449" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="450" ht="15.75" customHeight="1">
+      <c r="A450" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="451" ht="15.75" customHeight="1">
+      <c r="A451" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="452" ht="15.75" customHeight="1">
+      <c r="A452" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="453" ht="15.75" customHeight="1">
+      <c r="A453" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="454" ht="15.75" customHeight="1">
+      <c r="A454" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="455" ht="15.75" customHeight="1">
+      <c r="A455" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="456" ht="15.75" customHeight="1">
+      <c r="A456" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="457" ht="15.75" customHeight="1">
+      <c r="A457" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="458" ht="15.75" customHeight="1">
+      <c r="A458" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="459" ht="15.75" customHeight="1">
+      <c r="A459" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="460" ht="15.75" customHeight="1">
+      <c r="A460" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="461" ht="15.75" customHeight="1">
+      <c r="A461" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="462" ht="15.75" customHeight="1">
+      <c r="A462" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="463" ht="15.75" customHeight="1">
+      <c r="A463" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="464" ht="15.75" customHeight="1">
+      <c r="A464" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="465" ht="15.75" customHeight="1">
+      <c r="A465" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="466" ht="15.75" customHeight="1">
+      <c r="A466" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="467" ht="15.75" customHeight="1">
+      <c r="A467" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="468" ht="15.75" customHeight="1">
+      <c r="A468" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="469" ht="15.75" customHeight="1">
+      <c r="A469" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="470" ht="15.75" customHeight="1">
+      <c r="A470" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="471" ht="15.75" customHeight="1">
+      <c r="A471" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="472" ht="15.75" customHeight="1">
+      <c r="A472" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="473" ht="15.75" customHeight="1">
+      <c r="A473" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="474" ht="15.75" customHeight="1">
+      <c r="A474" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="475" ht="15.75" customHeight="1">
+      <c r="A475" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="476" ht="15.75" customHeight="1">
+      <c r="A476" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="477" ht="15.75" customHeight="1">
+      <c r="A477" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="478" ht="15.75" customHeight="1">
+      <c r="A478" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="479" ht="15.75" customHeight="1">
+      <c r="A479" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="480" ht="15.75" customHeight="1">
+      <c r="A480" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="481" ht="15.75" customHeight="1">
+      <c r="A481" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="482" ht="15.75" customHeight="1">
+      <c r="A482" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="483" ht="15.75" customHeight="1">
+      <c r="A483" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="484" ht="15.75" customHeight="1">
+      <c r="A484" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="485" ht="15.75" customHeight="1">
+      <c r="A485" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="486" ht="15.75" customHeight="1">
+      <c r="A486" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="487" ht="15.75" customHeight="1">
+      <c r="A487" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="488" ht="15.75" customHeight="1">
+      <c r="A488" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="489" ht="15.75" customHeight="1">
+      <c r="A489" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="490" ht="15.75" customHeight="1">
+      <c r="A490" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="491" ht="15.75" customHeight="1">
+      <c r="A491" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="492" ht="15.75" customHeight="1">
+      <c r="A492" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="493" ht="15.75" customHeight="1">
+      <c r="A493" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="494" ht="15.75" customHeight="1">
+      <c r="A494" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="495" ht="15.75" customHeight="1">
+      <c r="A495" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="496" ht="15.75" customHeight="1">
+      <c r="A496" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="497" ht="15.75" customHeight="1">
+      <c r="A497" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="498" ht="15.75" customHeight="1">
+      <c r="A498" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="499" ht="15.75" customHeight="1">
+      <c r="A499" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="500" ht="15.75" customHeight="1">
+      <c r="A500" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="501" ht="15.75" customHeight="1">
+      <c r="A501" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="502" ht="15.75" customHeight="1">
+      <c r="A502" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="503" ht="15.75" customHeight="1">
+      <c r="A503" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="504" ht="15.75" customHeight="1">
+      <c r="A504" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="505" ht="15.75" customHeight="1">
+      <c r="A505" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="506" ht="15.75" customHeight="1">
+      <c r="A506" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="507" ht="15.75" customHeight="1">
+      <c r="A507" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="508" ht="15.75" customHeight="1">
+      <c r="A508" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="509" ht="15.75" customHeight="1">
+      <c r="A509" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="510" ht="15.75" customHeight="1">
+      <c r="A510" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="511" ht="15.75" customHeight="1">
+      <c r="A511" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="512" ht="15.75" customHeight="1">
+      <c r="A512" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="513" ht="15.75" customHeight="1">
+      <c r="A513" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="514" ht="15.75" customHeight="1">
+      <c r="A514" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="515" ht="15.75" customHeight="1">
+      <c r="A515" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="516" ht="15.75" customHeight="1">
+      <c r="A516" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="517" ht="15.75" customHeight="1">
+      <c r="A517" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="518" ht="15.75" customHeight="1">
+      <c r="A518" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="519" ht="15.75" customHeight="1">
+      <c r="A519" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="520" ht="15.75" customHeight="1">
+      <c r="A520" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="521" ht="15.75" customHeight="1">
+      <c r="A521" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="522" ht="15.75" customHeight="1">
+      <c r="A522" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="523" ht="15.75" customHeight="1">
+      <c r="A523" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="524" ht="15.75" customHeight="1">
+      <c r="A524" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="525" ht="15.75" customHeight="1">
+      <c r="A525" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="526" ht="15.75" customHeight="1">
+      <c r="A526" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="527" ht="15.75" customHeight="1">
+      <c r="A527" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="528" ht="15.75" customHeight="1">
+      <c r="A528" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="529" ht="15.75" customHeight="1">
+      <c r="A529" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="530" ht="15.75" customHeight="1">
+      <c r="A530" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="531" ht="15.75" customHeight="1">
+      <c r="A531" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="532" ht="15.75" customHeight="1">
+      <c r="A532" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="533" ht="15.75" customHeight="1">
+      <c r="A533" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="534" ht="15.75" customHeight="1">
+      <c r="A534" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="535" ht="15.75" customHeight="1">
+      <c r="A535" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="536" ht="15.75" customHeight="1">
+      <c r="A536" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="537" ht="15.75" customHeight="1">
+      <c r="A537" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="538" ht="15.75" customHeight="1">
+      <c r="A538" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="539" ht="15.75" customHeight="1">
+      <c r="A539" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="540" ht="15.75" customHeight="1">
+      <c r="A540" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="541" ht="15.75" customHeight="1">
+      <c r="A541" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="542" ht="15.75" customHeight="1">
+      <c r="A542" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="543" ht="15.75" customHeight="1">
+      <c r="A543" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="544" ht="15.75" customHeight="1">
+      <c r="A544" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="545" ht="15.75" customHeight="1">
+      <c r="A545" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="546" ht="15.75" customHeight="1">
+      <c r="A546" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="547" ht="15.75" customHeight="1">
+      <c r="A547" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="548" ht="15.75" customHeight="1">
+      <c r="A548" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="549" ht="15.75" customHeight="1">
+      <c r="A549" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="550" ht="15.75" customHeight="1">
+      <c r="A550" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="551" ht="15.75" customHeight="1">
+      <c r="A551" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="552" ht="15.75" customHeight="1">
+      <c r="A552" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="553" ht="15.75" customHeight="1">
+      <c r="A553" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="554" ht="15.75" customHeight="1">
+      <c r="A554" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="555" ht="15.75" customHeight="1">
+      <c r="A555" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="556" ht="15.75" customHeight="1">
+      <c r="A556" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="557" ht="15.75" customHeight="1">
+      <c r="A557" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="558" ht="15.75" customHeight="1">
+      <c r="A558" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="559" ht="15.75" customHeight="1">
+      <c r="A559" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="560" ht="15.75" customHeight="1">
+      <c r="A560" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="561" ht="15.75" customHeight="1">
+      <c r="A561" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="562" ht="15.75" customHeight="1">
+      <c r="A562" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="563" ht="15.75" customHeight="1">
+      <c r="A563" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="564" ht="15.75" customHeight="1">
+      <c r="A564" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="565" ht="15.75" customHeight="1">
+      <c r="A565" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="566" ht="15.75" customHeight="1">
+      <c r="A566" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="567" ht="15.75" customHeight="1">
+      <c r="A567" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="568" ht="15.75" customHeight="1">
+      <c r="A568" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="569" ht="15.75" customHeight="1">
+      <c r="A569" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="570" ht="15.75" customHeight="1">
+      <c r="A570" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="571" ht="15.75" customHeight="1">
+      <c r="A571" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="572" ht="15.75" customHeight="1">
+      <c r="A572" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="573" ht="15.75" customHeight="1">
+      <c r="A573" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="574" ht="15.75" customHeight="1">
+      <c r="A574" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="575" ht="15.75" customHeight="1">
+      <c r="A575" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="576" ht="15.75" customHeight="1">
+      <c r="A576" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="577" ht="15.75" customHeight="1">
+      <c r="A577" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="578" ht="15.75" customHeight="1">
+      <c r="A578" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="579" ht="15.75" customHeight="1">
+      <c r="A579" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="580" ht="15.75" customHeight="1">
+      <c r="A580" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="581" ht="15.75" customHeight="1">
+      <c r="A581" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="582" ht="15.75" customHeight="1">
+      <c r="A582" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="583" ht="15.75" customHeight="1">
+      <c r="A583" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="584" ht="15.75" customHeight="1">
+      <c r="A584" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="585" ht="15.75" customHeight="1">
+      <c r="A585" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="586" ht="15.75" customHeight="1">
+      <c r="A586" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="587" ht="15.75" customHeight="1">
+      <c r="A587" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="588" ht="15.75" customHeight="1">
+      <c r="A588" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="589" ht="15.75" customHeight="1">
+      <c r="A589" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="590" ht="15.75" customHeight="1">
+      <c r="A590" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="591" ht="15.75" customHeight="1">
+      <c r="A591" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="592" ht="15.75" customHeight="1">
+      <c r="A592" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="593" ht="15.75" customHeight="1">
+      <c r="A593" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="594" ht="15.75" customHeight="1">
+      <c r="A594" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="595" ht="15.75" customHeight="1">
+      <c r="A595" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="596" ht="15.75" customHeight="1">
+      <c r="A596" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="597" ht="15.75" customHeight="1">
+      <c r="A597" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="598" ht="15.75" customHeight="1">
+      <c r="A598" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="599" ht="15.75" customHeight="1">
+      <c r="A599" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="600" ht="15.75" customHeight="1">
+      <c r="A600" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="601" ht="15.75" customHeight="1">
+      <c r="A601" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="602" ht="15.75" customHeight="1">
+      <c r="A602" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="603" ht="15.75" customHeight="1">
+      <c r="A603" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="604" ht="15.75" customHeight="1">
+      <c r="A604" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="605" ht="15.75" customHeight="1">
+      <c r="A605" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="606" ht="15.75" customHeight="1">
+      <c r="A606" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="607" ht="15.75" customHeight="1">
+      <c r="A607" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="608" ht="15.75" customHeight="1">
+      <c r="A608" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="609" ht="15.75" customHeight="1">
+      <c r="A609" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="610" ht="15.75" customHeight="1">
+      <c r="A610" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="611" ht="15.75" customHeight="1">
+      <c r="A611" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="612" ht="15.75" customHeight="1">
+      <c r="A612" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="613" ht="15.75" customHeight="1"/>
     <row r="614" ht="15.75" customHeight="1"/>
     <row r="615" ht="15.75" customHeight="1"/>

</xml_diff>